<commit_message>
09-01 cho ngay mai, chuan bi trong excel tempalte
</commit_message>
<xml_diff>
--- a/Theo dõi/T1 2026 02-01.xlsx
+++ b/Theo dõi/T1 2026 02-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duc Anh\Theo dõi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MINH HAI DRIVER\MinhHaiDriver2\Theo dõi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A4B614-8488-4B8A-96EE-7616193C6F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9D6E47-2F86-4865-899B-C0B57F3F1DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="439" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-01" sheetId="5" r:id="rId1"/>
@@ -21,27 +21,19 @@
     <sheet name="06-01" sheetId="10" r:id="rId6"/>
     <sheet name="07-01" sheetId="11" r:id="rId7"/>
     <sheet name="08-01" sheetId="12" r:id="rId8"/>
+    <sheet name="09-01" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="110">
   <si>
     <t>STT</t>
   </si>
@@ -368,6 +360,9 @@
   </si>
   <si>
     <t>0975 617 376</t>
+  </si>
+  <si>
+    <t>DOANH THU 09/01/2026</t>
   </si>
 </sst>
 </file>
@@ -825,6 +820,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -837,9 +835,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -847,7 +842,189 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="135">
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FF5B9BD5"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF9C0006"/>
+        <name val="Times New Roman"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <name val="Times New Roman"/>
@@ -2665,169 +2842,239 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10215</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>2954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>118704</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01362463-7AC2-4BA7-AC4F-6E808A298476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2402895" y="8826914"/>
+          <a:ext cx="2719070" cy="5609770"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}" name="Table1453" displayName="Table1453" ref="B6:M23" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}" name="Table1453" displayName="Table1453" ref="B6:M23" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M23" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{E4641425-2A19-4B49-9673-70283C00A0C9}" name="STT" dataDxfId="116" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{025A0EEF-1CDF-4C0C-B939-08C1DD0A727D}" name="HỌ TÊN" dataDxfId="115" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{6BCA469E-875E-4DB8-B8F1-4CEF36B099CF}" name="SDT" dataDxfId="114" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{D9F1E73A-B9F0-40EF-AFAA-8EA36E51E6E5}" name="CCCD" dataDxfId="113" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{14CA9924-9789-4C5A-9CF8-07EBE7D52A04}" name="ĐỊA CHỈ" dataDxfId="112" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{6C450420-5538-4DFE-9199-B536E9A8E96F}" name="BIỂN SỐ" dataDxfId="111" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{AC3D7AF1-8B94-4F38-AB66-E23F1838615A}" name="DOANH THU" dataDxfId="110" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{EFCE95F7-84BE-4DDC-8F47-D72FEE60EEAF}" name="THỰC LÃNH" dataDxfId="109" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{8C4F1F4F-862F-4F19-89BC-03E1A18529D1}" name="HÌNH THỨC" dataDxfId="108" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{C632D7F3-C2D1-4A7E-8E44-63D7A4528237}" name="BILL" dataDxfId="107" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{41EE3F26-FB65-4525-BED8-40D96AC73E16}" name="NOTE" dataDxfId="106" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{95690A3D-EBB8-4295-8DD1-172792A9523E}" name="TIME" dataDxfId="105" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{E4641425-2A19-4B49-9673-70283C00A0C9}" name="STT" dataDxfId="131" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{025A0EEF-1CDF-4C0C-B939-08C1DD0A727D}" name="HỌ TÊN" dataDxfId="130" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{6BCA469E-875E-4DB8-B8F1-4CEF36B099CF}" name="SDT" dataDxfId="129" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{D9F1E73A-B9F0-40EF-AFAA-8EA36E51E6E5}" name="CCCD" dataDxfId="128" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{14CA9924-9789-4C5A-9CF8-07EBE7D52A04}" name="ĐỊA CHỈ" dataDxfId="127" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{6C450420-5538-4DFE-9199-B536E9A8E96F}" name="BIỂN SỐ" dataDxfId="126" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{AC3D7AF1-8B94-4F38-AB66-E23F1838615A}" name="DOANH THU" dataDxfId="125" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{EFCE95F7-84BE-4DDC-8F47-D72FEE60EEAF}" name="THỰC LÃNH" dataDxfId="124" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{8C4F1F4F-862F-4F19-89BC-03E1A18529D1}" name="HÌNH THỨC" dataDxfId="123" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{C632D7F3-C2D1-4A7E-8E44-63D7A4528237}" name="BILL" dataDxfId="122" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{41EE3F26-FB65-4525-BED8-40D96AC73E16}" name="NOTE" dataDxfId="121" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{95690A3D-EBB8-4295-8DD1-172792A9523E}" name="TIME" dataDxfId="120" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0BE112E-9FFD-4DE3-AB43-DC2522DF0F97}" name="Table1452" displayName="Table1452" ref="B6:M24" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0BE112E-9FFD-4DE3-AB43-DC2522DF0F97}" name="Table1452" displayName="Table1452" ref="B6:M24" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A0647350-C5C2-4A5A-9CE6-9C91A4BF1448}" name="STT" dataDxfId="101" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{E5CB0A83-0EE8-4763-BEA5-F47D20895CEB}" name="HỌ TÊN" dataDxfId="100" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{55163D38-55AB-49C5-AFDB-11106B1FB5EA}" name="SDT" dataDxfId="99" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{9DEEAE65-0EE6-4FDE-B947-A5EF76C2BD87}" name="CCCD" dataDxfId="98" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{5AFA717A-7A2A-4331-928B-98CBBDCDA0A2}" name="ĐỊA CHỈ" dataDxfId="97" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{F2FCA384-1F8E-40F4-BB65-79B0B14C2A89}" name="BIỂN SỐ" dataDxfId="96" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{FAE54719-B24E-4B85-BE9E-FBF95DD0E092}" name="DOANH THU" dataDxfId="95" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{36C3D2A6-4BF9-4A93-AD0A-18E2598162BA}" name="THỰC LÃNH" dataDxfId="94" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{BE0DF11B-4989-41AA-BEA3-81D6A56606B1}" name="HÌNH THỨC" dataDxfId="93" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{E428066A-6A33-430A-95DD-8E25B28D626C}" name="BILL" dataDxfId="92" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{928FFCBD-7074-4A5E-93E9-512B6CDBAC46}" name="NOTE" dataDxfId="91" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{054F524A-B0EB-4441-9D2F-48D3D98CB664}" name="TIME" dataDxfId="90" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{A0647350-C5C2-4A5A-9CE6-9C91A4BF1448}" name="STT" dataDxfId="116" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{E5CB0A83-0EE8-4763-BEA5-F47D20895CEB}" name="HỌ TÊN" dataDxfId="115" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{55163D38-55AB-49C5-AFDB-11106B1FB5EA}" name="SDT" dataDxfId="114" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{9DEEAE65-0EE6-4FDE-B947-A5EF76C2BD87}" name="CCCD" dataDxfId="113" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{5AFA717A-7A2A-4331-928B-98CBBDCDA0A2}" name="ĐỊA CHỈ" dataDxfId="112" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{F2FCA384-1F8E-40F4-BB65-79B0B14C2A89}" name="BIỂN SỐ" dataDxfId="111" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{FAE54719-B24E-4B85-BE9E-FBF95DD0E092}" name="DOANH THU" dataDxfId="110" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{36C3D2A6-4BF9-4A93-AD0A-18E2598162BA}" name="THỰC LÃNH" dataDxfId="109" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{BE0DF11B-4989-41AA-BEA3-81D6A56606B1}" name="HÌNH THỨC" dataDxfId="108" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{E428066A-6A33-430A-95DD-8E25B28D626C}" name="BILL" dataDxfId="107" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{928FFCBD-7074-4A5E-93E9-512B6CDBAC46}" name="NOTE" dataDxfId="106" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{054F524A-B0EB-4441-9D2F-48D3D98CB664}" name="TIME" dataDxfId="105" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{811EE2EE-55E9-4D50-8E60-6BD69129A816}" name="Table14524" displayName="Table14524" ref="B6:M24" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{811EE2EE-55E9-4D50-8E60-6BD69129A816}" name="Table14524" displayName="Table14524" ref="B6:M24" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{984C32DA-9CD0-4E13-B865-6EAED834D984}" name="STT" dataDxfId="86" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{F1DCB155-1D62-4027-A3DA-A9FBDBBDFC4D}" name="HỌ TÊN" dataDxfId="85" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{5C330DB0-1E19-466E-AB2C-E562D46DC243}" name="SDT" dataDxfId="84" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{AB7FBF00-4E37-4D6D-A82A-571965487148}" name="CCCD" dataDxfId="83" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{25AD663F-C9DC-45FA-87E3-EC98289C695D}" name="ĐỊA CHỈ" dataDxfId="82" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{0C05E7D7-64B8-43E4-BC46-95EB52EF87B4}" name="BIỂN SỐ" dataDxfId="81" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{DCE2CCF7-5F06-4F7F-8168-BF276332F656}" name="DOANH THU" dataDxfId="80" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{D07BFE34-76E9-4F19-A23E-07516BD1AFC9}" name="THỰC LÃNH" dataDxfId="79" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{F536DCC4-4F00-4248-B00E-1B801BDDEBBD}" name="HÌNH THỨC" dataDxfId="78" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{E474DC06-F263-48D8-BAD2-21F369101CD6}" name="BILL" dataDxfId="77" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{569676A8-F060-4B81-9319-D9A824EB8B46}" name="NOTE" dataDxfId="76" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{4C9FE953-00AF-4D77-B446-CBEC0FFE32D6}" name="TIME" dataDxfId="75" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{984C32DA-9CD0-4E13-B865-6EAED834D984}" name="STT" dataDxfId="101" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{F1DCB155-1D62-4027-A3DA-A9FBDBBDFC4D}" name="HỌ TÊN" dataDxfId="100" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{5C330DB0-1E19-466E-AB2C-E562D46DC243}" name="SDT" dataDxfId="99" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{AB7FBF00-4E37-4D6D-A82A-571965487148}" name="CCCD" dataDxfId="98" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{25AD663F-C9DC-45FA-87E3-EC98289C695D}" name="ĐỊA CHỈ" dataDxfId="97" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{0C05E7D7-64B8-43E4-BC46-95EB52EF87B4}" name="BIỂN SỐ" dataDxfId="96" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{DCE2CCF7-5F06-4F7F-8168-BF276332F656}" name="DOANH THU" dataDxfId="95" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{D07BFE34-76E9-4F19-A23E-07516BD1AFC9}" name="THỰC LÃNH" dataDxfId="94" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{F536DCC4-4F00-4248-B00E-1B801BDDEBBD}" name="HÌNH THỨC" dataDxfId="93" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{E474DC06-F263-48D8-BAD2-21F369101CD6}" name="BILL" dataDxfId="92" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{569676A8-F060-4B81-9319-D9A824EB8B46}" name="NOTE" dataDxfId="91" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{4C9FE953-00AF-4D77-B446-CBEC0FFE32D6}" name="TIME" dataDxfId="90" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49B02BE1-C610-460C-B461-D64E7BB29649}" name="Table145245" displayName="Table145245" ref="B6:M24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49B02BE1-C610-460C-B461-D64E7BB29649}" name="Table145245" displayName="Table145245" ref="B6:M24" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{DF404508-0107-419A-8FEC-EFB55BF001F1}" name="STT" dataDxfId="71" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{2D3FD697-D6D5-47C8-8441-D73D89975778}" name="HỌ TÊN" dataDxfId="70" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{E973C6FC-7D49-4C09-A7B8-491118C8F7ED}" name="SDT" dataDxfId="69" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{99802D82-09B1-4FB0-9F42-DB0D0E4E1880}" name="CCCD" dataDxfId="68" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{545E75FC-89EF-4EBD-8E8A-E21A7C5DD983}" name="ĐỊA CHỈ" dataDxfId="67" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{C61AD627-F01B-49BC-BE72-C4BA72782E0C}" name="BIỂN SỐ" dataDxfId="66" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{F71F42D2-0017-499B-BD73-6CA3452798B2}" name="DOANH THU" dataDxfId="65" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{17E776BC-FFDB-49A9-BA7F-F74CA3FA1E79}" name="THỰC LÃNH" dataDxfId="64" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{83DA542A-3997-424B-A7B2-D25B6B1B1F4A}" name="HÌNH THỨC" dataDxfId="63" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{94F40CAA-EBD9-440E-B930-2150A3120D38}" name="BILL" dataDxfId="62" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{6AB0CF3E-D0A0-4DAB-B8CE-54B1CB07881A}" name="NOTE" dataDxfId="61" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{2C692775-6E51-48EE-92EB-4FB2B57D99B9}" name="TIME" dataDxfId="60" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{DF404508-0107-419A-8FEC-EFB55BF001F1}" name="STT" dataDxfId="86" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{2D3FD697-D6D5-47C8-8441-D73D89975778}" name="HỌ TÊN" dataDxfId="85" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{E973C6FC-7D49-4C09-A7B8-491118C8F7ED}" name="SDT" dataDxfId="84" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{99802D82-09B1-4FB0-9F42-DB0D0E4E1880}" name="CCCD" dataDxfId="83" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{545E75FC-89EF-4EBD-8E8A-E21A7C5DD983}" name="ĐỊA CHỈ" dataDxfId="82" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{C61AD627-F01B-49BC-BE72-C4BA72782E0C}" name="BIỂN SỐ" dataDxfId="81" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{F71F42D2-0017-499B-BD73-6CA3452798B2}" name="DOANH THU" dataDxfId="80" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{17E776BC-FFDB-49A9-BA7F-F74CA3FA1E79}" name="THỰC LÃNH" dataDxfId="79" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{83DA542A-3997-424B-A7B2-D25B6B1B1F4A}" name="HÌNH THỨC" dataDxfId="78" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{94F40CAA-EBD9-440E-B930-2150A3120D38}" name="BILL" dataDxfId="77" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{6AB0CF3E-D0A0-4DAB-B8CE-54B1CB07881A}" name="NOTE" dataDxfId="76" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{2C692775-6E51-48EE-92EB-4FB2B57D99B9}" name="TIME" dataDxfId="75" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6D51770-D13F-4F99-B376-86240AE4A636}" name="Table1452456" displayName="Table1452456" ref="B6:M24" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6D51770-D13F-4F99-B376-86240AE4A636}" name="Table1452456" displayName="Table1452456" ref="B6:M24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{021C7381-52B0-487C-BDC0-1BFAE6723B42}" name="STT" dataDxfId="56" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{FCC93C85-2562-4DEC-8FE4-78554E01B098}" name="HỌ TÊN" dataDxfId="55" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{CBAF7620-956C-46F1-B90E-FF881C020840}" name="SDT" dataDxfId="54" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{5AA80C72-14CD-4ECA-B274-7E6DB4C710F0}" name="CCCD" dataDxfId="53" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{BBDC8231-A509-4F67-9641-21E894B6F3BB}" name="ĐỊA CHỈ" dataDxfId="52" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{4E5C67CA-7F62-46A7-B67B-D1F0D77BC2D0}" name="BIỂN SỐ" dataDxfId="51" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{7828CFFD-4ACF-4B8C-87C1-9BA98BDD2B3B}" name="DOANH THU" dataDxfId="50" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{C4C0E649-5B5C-4262-A054-DC4554985799}" name="THỰC LÃNH" dataDxfId="49" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{246DAA9C-7CDE-43CE-A7E0-A306769DE0F8}" name="HÌNH THỨC" dataDxfId="48" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{FEAFBFBE-1AF4-43B8-891C-A417A9898E29}" name="BILL" dataDxfId="47" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{74D4B397-CBE7-4110-8F80-F23CDA73BBFE}" name="NOTE" dataDxfId="46" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{BF91805E-61E6-49C9-9C35-3B13279CADD4}" name="TIME" dataDxfId="45" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{021C7381-52B0-487C-BDC0-1BFAE6723B42}" name="STT" dataDxfId="71" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{FCC93C85-2562-4DEC-8FE4-78554E01B098}" name="HỌ TÊN" dataDxfId="70" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{CBAF7620-956C-46F1-B90E-FF881C020840}" name="SDT" dataDxfId="69" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{5AA80C72-14CD-4ECA-B274-7E6DB4C710F0}" name="CCCD" dataDxfId="68" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{BBDC8231-A509-4F67-9641-21E894B6F3BB}" name="ĐỊA CHỈ" dataDxfId="67" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{4E5C67CA-7F62-46A7-B67B-D1F0D77BC2D0}" name="BIỂN SỐ" dataDxfId="66" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{7828CFFD-4ACF-4B8C-87C1-9BA98BDD2B3B}" name="DOANH THU" dataDxfId="65" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{C4C0E649-5B5C-4262-A054-DC4554985799}" name="THỰC LÃNH" dataDxfId="64" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{246DAA9C-7CDE-43CE-A7E0-A306769DE0F8}" name="HÌNH THỨC" dataDxfId="63" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{FEAFBFBE-1AF4-43B8-891C-A417A9898E29}" name="BILL" dataDxfId="62" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{74D4B397-CBE7-4110-8F80-F23CDA73BBFE}" name="NOTE" dataDxfId="61" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{BF91805E-61E6-49C9-9C35-3B13279CADD4}" name="TIME" dataDxfId="60" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{704C3A58-D406-453F-8AC1-A5B4A47BB0C4}" name="Table14524567" displayName="Table14524567" ref="B6:M24" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{704C3A58-D406-453F-8AC1-A5B4A47BB0C4}" name="Table14524567" displayName="Table14524567" ref="B6:M24" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{395E0AEF-65DD-4F52-8E14-3F35D9FC3368}" name="STT" dataDxfId="41" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{9AE4DC19-F9B6-43F0-A90F-B4F19B4ECECB}" name="HỌ TÊN" dataDxfId="40" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{F2807F19-50E8-43E8-AAA8-2736AB34EA40}" name="SDT" dataDxfId="39" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{A9CAB30F-7177-438D-BC24-B95AE3E4F2E1}" name="CCCD" dataDxfId="38" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{79CCA633-E92E-4399-8A6F-9187CFA8C624}" name="ĐỊA CHỈ" dataDxfId="37" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{920798EF-484E-41FD-B789-6C522DE8129F}" name="BIỂN SỐ" dataDxfId="36" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{E1C353DD-B746-4FDC-8D04-BDA2D046D60D}" name="DOANH THU" dataDxfId="35" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{9C97F9DB-7299-4176-861A-6A82D87978B7}" name="THỰC LÃNH" dataDxfId="34" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{DE161CA4-4F2C-42F2-ACFF-92650F7DAAEB}" name="HÌNH THỨC" dataDxfId="33" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{96EECF95-D222-4AB7-920D-12768887EF5B}" name="BILL" dataDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{39B7E33C-421D-41BB-9FB6-ECF9EB938AB4}" name="NOTE" dataDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{83A24DE4-F137-463F-9772-3D3919BAE1E9}" name="TIME" dataDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{395E0AEF-65DD-4F52-8E14-3F35D9FC3368}" name="STT" dataDxfId="56" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{9AE4DC19-F9B6-43F0-A90F-B4F19B4ECECB}" name="HỌ TÊN" dataDxfId="55" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{F2807F19-50E8-43E8-AAA8-2736AB34EA40}" name="SDT" dataDxfId="54" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{A9CAB30F-7177-438D-BC24-B95AE3E4F2E1}" name="CCCD" dataDxfId="53" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{79CCA633-E92E-4399-8A6F-9187CFA8C624}" name="ĐỊA CHỈ" dataDxfId="52" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{920798EF-484E-41FD-B789-6C522DE8129F}" name="BIỂN SỐ" dataDxfId="51" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{E1C353DD-B746-4FDC-8D04-BDA2D046D60D}" name="DOANH THU" dataDxfId="50" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{9C97F9DB-7299-4176-861A-6A82D87978B7}" name="THỰC LÃNH" dataDxfId="49" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{DE161CA4-4F2C-42F2-ACFF-92650F7DAAEB}" name="HÌNH THỨC" dataDxfId="48" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{96EECF95-D222-4AB7-920D-12768887EF5B}" name="BILL" dataDxfId="47" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{39B7E33C-421D-41BB-9FB6-ECF9EB938AB4}" name="NOTE" dataDxfId="46" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{83A24DE4-F137-463F-9772-3D3919BAE1E9}" name="TIME" dataDxfId="45" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{500679E0-EE2D-4EE0-8D49-BD93EAE287BF}" name="Table145245678" displayName="Table145245678" ref="B6:M24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{500679E0-EE2D-4EE0-8D49-BD93EAE287BF}" name="Table145245678" displayName="Table145245678" ref="B6:M24" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{FE5E9CEF-58C1-4672-8B6E-C5046C4F970F}" name="STT" dataDxfId="26" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{A2DA5362-86C1-4D95-969F-62FCF30900C9}" name="HỌ TÊN" dataDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{8B1983FB-CAD9-4F22-8DE7-E134AE6A9F70}" name="SDT" dataDxfId="24" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{498B51D9-B2C9-4D7B-BBBD-082B2067379C}" name="CCCD" dataDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{C63756CC-CCDE-4370-8B2E-B494A7DC813D}" name="ĐỊA CHỈ" dataDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{6B166947-75EF-4D67-92F8-79B3BFFB2F5E}" name="BIỂN SỐ" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{133865C5-3727-420D-8494-5560F77B5277}" name="DOANH THU" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{2270A241-369C-4D02-A8E4-2AAB5F44362E}" name="THỰC LÃNH" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{45C5A9A4-B5C2-4DE5-B6E1-557D6B332D47}" name="HÌNH THỨC" dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{8CB9BE29-AE4B-4972-B577-50C9BE6F5188}" name="BILL" dataDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{D6FC356D-48E7-4DA9-B7CD-69A2C3E105E5}" name="NOTE" dataDxfId="16" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{EC0104D6-C23A-4791-8BD0-03B669770D6D}" name="TIME" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{FE5E9CEF-58C1-4672-8B6E-C5046C4F970F}" name="STT" dataDxfId="41" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{A2DA5362-86C1-4D95-969F-62FCF30900C9}" name="HỌ TÊN" dataDxfId="40" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{8B1983FB-CAD9-4F22-8DE7-E134AE6A9F70}" name="SDT" dataDxfId="39" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{498B51D9-B2C9-4D7B-BBBD-082B2067379C}" name="CCCD" dataDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{C63756CC-CCDE-4370-8B2E-B494A7DC813D}" name="ĐỊA CHỈ" dataDxfId="37" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{6B166947-75EF-4D67-92F8-79B3BFFB2F5E}" name="BIỂN SỐ" dataDxfId="36" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{133865C5-3727-420D-8494-5560F77B5277}" name="DOANH THU" dataDxfId="35" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{2270A241-369C-4D02-A8E4-2AAB5F44362E}" name="THỰC LÃNH" dataDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{45C5A9A4-B5C2-4DE5-B6E1-557D6B332D47}" name="HÌNH THỨC" dataDxfId="33" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{8CB9BE29-AE4B-4972-B577-50C9BE6F5188}" name="BILL" dataDxfId="32" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{D6FC356D-48E7-4DA9-B7CD-69A2C3E105E5}" name="NOTE" dataDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{EC0104D6-C23A-4791-8BD0-03B669770D6D}" name="TIME" dataDxfId="30" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F6B294FA-FBE8-4560-9B90-DC686FD21438}" name="Table1452456789" displayName="Table1452456789" ref="B6:M24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Bad" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F6B294FA-FBE8-4560-9B90-DC686FD21438}" name="Table1452456789" displayName="Table1452456789" ref="B6:M24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Bad" dataCellStyle="Normal">
   <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{AF0208C4-E4FE-4DFD-BAF4-BF1165EEA465}" name="STT" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{CDE784D9-BEC1-45FE-9CFA-FBFFA9772F9D}" name="HỌ TÊN" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{3F06EBB4-066C-4D70-BCDB-6385DD5521D0}" name="SDT" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{6716FF64-CBA6-41E2-AC66-8E6674578FB1}" name="CCCD" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{E9AF3165-7AF3-4802-8A2B-C4778B4E6C54}" name="ĐỊA CHỈ" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{68CEAC9B-947C-49B6-A2BB-6DE884DDEBFB}" name="BIỂN SỐ" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{4F868D74-6BC9-4BE1-B4C6-159BCF2EDA47}" name="DOANH THU" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="8" xr3:uid="{D5E9904F-827E-445C-B51C-F330CC45F31E}" name="THỰC LÃNH" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="9" xr3:uid="{11E0E58A-8F57-4240-A051-39E671386B4D}" name="HÌNH THỨC" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="10" xr3:uid="{1CB6152F-EB83-4348-AC14-5DFBE58A8396}" name="BILL" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{94A817A4-0B58-40F9-974C-34BF9DC3FEC2}" name="NOTE" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{31980D75-0507-4AF0-9CE2-8238A4185BB5}" name="TIME" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{AF0208C4-E4FE-4DFD-BAF4-BF1165EEA465}" name="STT" dataDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{CDE784D9-BEC1-45FE-9CFA-FBFFA9772F9D}" name="HỌ TÊN" dataDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{3F06EBB4-066C-4D70-BCDB-6385DD5521D0}" name="SDT" dataDxfId="24" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{6716FF64-CBA6-41E2-AC66-8E6674578FB1}" name="CCCD" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{E9AF3165-7AF3-4802-8A2B-C4778B4E6C54}" name="ĐỊA CHỈ" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{68CEAC9B-947C-49B6-A2BB-6DE884DDEBFB}" name="BIỂN SỐ" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{4F868D74-6BC9-4BE1-B4C6-159BCF2EDA47}" name="DOANH THU" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{D5E9904F-827E-445C-B51C-F330CC45F31E}" name="THỰC LÃNH" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{11E0E58A-8F57-4240-A051-39E671386B4D}" name="HÌNH THỨC" dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{1CB6152F-EB83-4348-AC14-5DFBE58A8396}" name="BILL" dataDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{94A817A4-0B58-40F9-974C-34BF9DC3FEC2}" name="NOTE" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{31980D75-0507-4AF0-9CE2-8238A4185BB5}" name="TIME" dataDxfId="15" dataCellStyle="Normal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D2417A03-54AF-4CD5-ACE5-D93CFF57121A}" name="Table145245678910" displayName="Table145245678910" ref="B6:M24" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12" headerRowCellStyle="Bad" dataCellStyle="Normal">
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{46F63323-68E0-4510-BA08-C9DB0457E239}" name="STT" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{DFFE4649-68A2-46AF-9EB2-F9BCC12F0326}" name="HỌ TÊN" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{044325E6-629C-47E6-AD1F-1668BE3F6282}" name="SDT" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{EBF1E448-4F61-4D59-A0A4-4A4CD1B729A0}" name="CCCD" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{61DE7A23-28E7-447B-BC88-192F90C3530C}" name="ĐỊA CHỈ" dataDxfId="7" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{FB3C372D-64BB-4DE7-9784-B0486D1440AE}" name="BIỂN SỐ" dataDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{8E94CCD3-47C5-495A-8218-D190EA4CC0F9}" name="DOANH THU" dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="8" xr3:uid="{A2A5BB41-6A08-4052-8051-0822BDE7DF81}" name="THỰC LÃNH" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{B22F578A-3E37-45C7-921C-CE20D5830508}" name="HÌNH THỨC" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{84F487C4-8284-4D17-8D43-13F61D066D7B}" name="BILL" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{5178B337-902A-48D7-96F7-964B735DEEC3}" name="NOTE" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{C25FF628-EA2A-4D04-B390-A6CA292E6FF9}" name="TIME" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3103,56 +3350,56 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3437,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -3224,7 +3471,7 @@
       </c>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B23" si="0">B7 +1</f>
         <v>2</v>
@@ -3257,7 +3504,7 @@
       <c r="L8" s="27"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3291,7 +3538,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3325,7 +3572,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3359,7 +3606,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3393,7 +3640,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3426,7 +3673,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3460,7 +3707,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3494,7 +3741,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3528,7 +3775,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3562,7 +3809,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3596,7 +3843,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3630,7 +3877,7 @@
       <c r="L19" s="32"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3647,7 +3894,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3664,7 +3911,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3686,7 +3933,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3708,7 +3955,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="25" spans="2:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D25" s="23" t="s">
         <v>65</v>
       </c>
@@ -3718,20 +3965,20 @@
       <c r="F25" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="H25" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="53"/>
+      <c r="I25" s="54"/>
       <c r="J25" s="9">
         <f>SUM(H7:H1000)</f>
         <v>24820000</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H26" s="53" t="s">
+    <row r="26" spans="2:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H26" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(I7:I1000)</f>
         <v>14390000</v>
@@ -3742,67 +3989,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B43" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="21" t="s">
         <v>35</v>
       </c>
@@ -3832,56 +4079,56 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +4166,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -3951,7 +4198,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f>B7 +1</f>
         <v>2</v>
@@ -3987,7 +4234,7 @@
       <c r="L8" s="35"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -4020,7 +4267,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B24" si="0">B9 +1</f>
         <v>4</v>
@@ -4054,7 +4301,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4090,7 +4337,7 @@
       <c r="L11" s="35"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4124,7 +4371,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4160,7 +4407,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4194,7 +4441,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4228,7 +4475,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4262,7 +4509,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4295,7 +4542,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -4330,7 +4577,7 @@
       <c r="L18" s="35"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4363,7 +4610,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>71</v>
       </c>
@@ -4399,7 +4646,7 @@
       <c r="L20" s="35"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>71</v>
       </c>
@@ -4436,7 +4683,7 @@
       <c r="L21" s="35"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4469,7 +4716,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4502,7 +4749,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -4535,7 +4782,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -4545,20 +4792,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>29135000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>17346000</v>
@@ -4574,67 +4821,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -4665,56 +4912,56 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -4752,7 +4999,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -4784,7 +5031,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f>B7 +1</f>
         <v>2</v>
@@ -4819,7 +5066,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -4852,7 +5099,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B24" si="0">B9 +1</f>
         <v>4</v>
@@ -4888,7 +5135,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4924,7 +5171,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4958,7 +5205,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4994,7 +5241,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5027,7 +5274,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5061,7 +5308,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5095,7 +5342,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5129,7 +5376,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5164,7 +5411,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5197,7 +5444,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -5231,7 +5478,7 @@
       <c r="L20" s="43"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f>B20 +1</f>
@@ -5265,7 +5512,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5298,7 +5545,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5331,7 +5578,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5364,7 +5611,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -5374,20 +5621,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>32170000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>19075000</v>
@@ -5403,67 +5650,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -5493,56 +5740,56 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -5580,7 +5827,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -5613,7 +5860,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f>B7 +1</f>
         <v>2</v>
@@ -5649,7 +5896,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -5682,7 +5929,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B23" si="0">B9 +1</f>
         <v>4</v>
@@ -5717,7 +5964,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -5753,7 +6000,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5787,7 +6034,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5823,7 +6070,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5857,7 +6104,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5891,7 +6138,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5925,7 +6172,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5959,7 +6206,7 @@
       <c r="L17" s="2"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -5997,7 +6244,7 @@
       </c>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6031,7 +6278,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -6065,7 +6312,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f>B20 +1</f>
@@ -6099,7 +6346,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6132,7 +6379,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6165,7 +6412,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -6179,7 +6426,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -6189,20 +6436,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>30806000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>18342000</v>
@@ -6218,67 +6465,67 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -6308,56 +6555,56 @@
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -6395,7 +6642,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -6427,7 +6674,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B23" si="0">B7 +1</f>
         <v>2</v>
@@ -6463,7 +6710,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6496,7 +6743,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6532,7 +6779,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6568,7 +6815,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6602,7 +6849,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6637,7 +6884,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6671,7 +6918,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6705,7 +6952,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6738,7 +6985,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6772,7 +7019,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -6807,7 +7054,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6840,7 +7087,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -6874,7 +7121,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -6909,7 +7156,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6942,7 +7189,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6975,7 +7222,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -6989,7 +7236,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -6999,20 +7246,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>30762000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>18280000</v>
@@ -7028,22 +7275,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
@@ -7051,47 +7298,47 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -7121,56 +7368,56 @@
       <selection activeCell="I7" sqref="I7:I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -7208,7 +7455,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -7241,7 +7488,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B23" si="0">B7 +1</f>
         <v>2</v>
@@ -7277,7 +7524,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7311,7 +7558,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7347,7 +7594,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7383,7 +7630,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7417,7 +7664,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7453,7 +7700,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7487,7 +7734,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7521,7 +7768,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7555,7 +7802,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7590,7 +7837,7 @@
       </c>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7626,7 +7873,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7659,7 +7906,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -7693,7 +7940,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -7728,7 +7975,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7761,7 +8008,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7794,7 +8041,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -7808,7 +8055,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -7818,20 +8065,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>31566000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>18200000</v>
@@ -7847,22 +8094,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
@@ -7870,47 +8117,47 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -7940,56 +8187,56 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:13" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:13" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -8027,7 +8274,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -8060,7 +8307,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B23" si="0">B7 +1</f>
         <v>2</v>
@@ -8096,7 +8343,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8130,7 +8377,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8166,7 +8413,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8202,7 +8449,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8236,7 +8483,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8272,7 +8519,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8306,7 +8553,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8340,7 +8587,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8374,7 +8621,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8406,7 +8653,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -8442,7 +8689,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8476,7 +8723,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -8510,7 +8757,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -8545,7 +8792,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8579,7 +8826,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8612,7 +8859,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -8626,7 +8873,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -8636,20 +8883,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>31500000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>18630000</v>
@@ -8665,22 +8912,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
@@ -8688,47 +8935,47 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
@@ -8754,62 +9001,62 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A5" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.109375" style="1"/>
+    <col min="16" max="16" width="16.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:16" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:16" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J4" s="26"/>
     </row>
-    <row r="6" spans="2:16" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
@@ -8850,7 +9097,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -8885,7 +9132,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B23" si="0">B7 +1</f>
         <v>2</v>
@@ -8924,7 +9171,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8958,7 +9205,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8994,7 +9241,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -9030,7 +9277,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -9064,7 +9311,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -9100,7 +9347,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -9134,7 +9381,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -9168,7 +9415,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -9202,7 +9449,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9213,7 +9460,7 @@
       <c r="D17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="50">
         <v>91085001515</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -9235,7 +9482,7 @@
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -9271,7 +9518,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9305,7 +9552,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -9339,7 +9586,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -9367,14 +9614,14 @@
         <f t="shared" si="1"/>
         <v>2286000</v>
       </c>
-      <c r="J21" s="45" t="s">
-        <v>72</v>
+      <c r="J21" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -9408,7 +9655,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -9442,7 +9689,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -9456,7 +9703,7 @@
       <c r="L24" s="2"/>
       <c r="M24" s="12"/>
     </row>
-    <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
       <c r="D26" s="23" t="s">
         <v>65</v>
       </c>
@@ -9466,20 +9713,20 @@
       <c r="F26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="53" t="s">
+      <c r="H26" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="54"/>
       <c r="J26" s="9">
         <f>SUM(H7:H1001)</f>
         <v>32130000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="H27" s="53" t="s">
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
         <v>19110000</v>
@@ -9495,22 +9742,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B44" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B46" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B47" s="18" t="s">
         <v>48</v>
       </c>
@@ -9518,62 +9765,820 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B48" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B49" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B50" s="20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B51" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B52" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B53" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B54" s="20" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B55" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B56" s="21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B57" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="2:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B548C305-7CC5-4E0E-A313-9D8AB40EB321}">
+  <dimension ref="A2:P59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="21" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.109375" style="1"/>
+    <col min="16" max="16" width="16.88671875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="2:16" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J4" s="26"/>
+    </row>
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="B6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4">
+        <v>38096003688</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="P7" s="47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <f t="shared" ref="B8:B23" si="0">B7 +1</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>91203011680</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="P8" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
+        <v>89078016404</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+    </row>
+    <row r="10" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4">
+        <v>89099008054</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="11" spans="2:16" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>91088020664</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+    </row>
+    <row r="12" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="8">
+        <v>89082022656</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8">
+        <v>42088019031</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="8">
+        <v>49202008987</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="13"/>
+    </row>
+    <row r="15" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8">
+        <v>93097001330</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="2:16" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="8">
+        <v>95095009661</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="50">
+        <v>91085001515</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="8">
+        <v>42094001136</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="8">
+        <v>38085004911</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="35"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="3">
+        <v>70081001153</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="3">
+        <v>27068001194</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:13" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="12"/>
+    </row>
+    <row r="26" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="D26" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="54"/>
+      <c r="J26" s="9">
+        <f>SUM(H7:H1001)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="54"/>
+      <c r="J27" s="9">
+        <f>SUM(I7:I1001)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B44" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B45" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B47" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B49" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B50" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B52" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B53" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B54" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B55" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B56" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="B57" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:K2"/>

</xml_diff>

<commit_message>
09-01 da chinh sua anh dat vao ngay 07 tu 558 xuong con 540 do sai sot tien mat
</commit_message>
<xml_diff>
--- a/Theo dõi/T1 2026 02-01.xlsx
+++ b/Theo dõi/T1 2026 02-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Duc Anh\Theo dõi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728A953-6CAA-4CBD-BDA0-64A6A3E1BC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC5DEE7-EE71-4474-9198-B8FD9D5D2962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="439" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01-01" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="116">
   <si>
     <t>STT</t>
   </si>
@@ -345,12 +345,6 @@
     <t>DOANH THU 07/01/2026</t>
   </si>
   <si>
-    <t>ĐẠT</t>
-  </si>
-  <si>
-    <t>BÁC THAO</t>
-  </si>
-  <si>
     <t>DOANH THU 08/01/2026</t>
   </si>
   <si>
@@ -385,6 +379,19 @@
   </si>
   <si>
     <t>HUỲNH HOÀNG VŨ (Sun)</t>
+  </si>
+  <si>
+    <t>QUANG HÀ (Vin)</t>
+  </si>
+  <si>
+    <t>ĐẠT (Vin)</t>
+  </si>
+  <si>
+    <t>BÁC THAO (Vin)</t>
+  </si>
+  <si>
+    <t>Đức anh nhận 
+chuyển khoản</t>
   </si>
 </sst>
 </file>
@@ -707,7 +714,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -886,6 +893,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2991,7 +3001,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>16565</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>185939</xdr:rowOff>
+      <xdr:rowOff>185940</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3176,7 +3186,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}" name="Table1453" displayName="Table1453" ref="B6:M23" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148" tableBorderDxfId="147" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M23" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}"/>
+  <autoFilter ref="B6:M23" xr:uid="{8259D2E9-CBBA-448C-8826-9D32D86A1C8E}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{E4641425-2A19-4B49-9673-70283C00A0C9}" name="STT" dataDxfId="146" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{025A0EEF-1CDF-4C0C-B939-08C1DD0A727D}" name="HỌ TÊN" dataDxfId="145" dataCellStyle="Normal"/>
@@ -3220,7 +3236,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0BE112E-9FFD-4DE3-AB43-DC2522DF0F97}" name="Table1452" displayName="Table1452" ref="B6:M24" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133" tableBorderDxfId="132" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{A0647350-C5C2-4A5A-9CE6-9C91A4BF1448}" name="STT" dataDxfId="131" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{E5CB0A83-0EE8-4763-BEA5-F47D20895CEB}" name="HỌ TÊN" dataDxfId="130" dataCellStyle="Normal"/>
@@ -3241,7 +3263,13 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{811EE2EE-55E9-4D50-8E60-6BD69129A816}" name="Table14524" displayName="Table14524" ref="B6:M24" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118" tableBorderDxfId="117" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{984C32DA-9CD0-4E13-B865-6EAED834D984}" name="STT" dataDxfId="116" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{F1DCB155-1D62-4027-A3DA-A9FBDBBDFC4D}" name="HỌ TÊN" dataDxfId="115" dataCellStyle="Normal"/>
@@ -3262,7 +3290,13 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{49B02BE1-C610-460C-B461-D64E7BB29649}" name="Table145245" displayName="Table145245" ref="B6:M24" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{DF404508-0107-419A-8FEC-EFB55BF001F1}" name="STT" dataDxfId="101" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{2D3FD697-D6D5-47C8-8441-D73D89975778}" name="HỌ TÊN" dataDxfId="100" dataCellStyle="Normal"/>
@@ -3283,7 +3317,13 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6D51770-D13F-4F99-B376-86240AE4A636}" name="Table1452456" displayName="Table1452456" ref="B6:M24" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{021C7381-52B0-487C-BDC0-1BFAE6723B42}" name="STT" dataDxfId="86" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{FCC93C85-2562-4DEC-8FE4-78554E01B098}" name="HỌ TÊN" dataDxfId="85" dataCellStyle="Normal"/>
@@ -3304,7 +3344,13 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{704C3A58-D406-453F-8AC1-A5B4A47BB0C4}" name="Table14524567" displayName="Table14524567" ref="B6:M24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{395E0AEF-65DD-4F52-8E14-3F35D9FC3368}" name="STT" dataDxfId="71" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{9AE4DC19-F9B6-43F0-A90F-B4F19B4ECECB}" name="HỌ TÊN" dataDxfId="70" dataCellStyle="Normal"/>
@@ -3325,7 +3371,13 @@
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{500679E0-EE2D-4EE0-8D49-BD93EAE287BF}" name="Table145245678" displayName="Table145245678" ref="B6:M24" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*(Vin)*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{FE5E9CEF-58C1-4672-8B6E-C5046C4F970F}" name="STT" dataDxfId="56" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{A2DA5362-86C1-4D95-969F-62FCF30900C9}" name="HỌ TÊN" dataDxfId="55" dataCellStyle="Normal"/>
@@ -3346,7 +3398,13 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F6B294FA-FBE8-4560-9B90-DC686FD21438}" name="Table1452456789" displayName="Table1452456789" ref="B6:M24" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" tableBorderDxfId="42" headerRowCellStyle="Bad" dataCellStyle="Normal">
-  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}"/>
+  <autoFilter ref="B6:M24" xr:uid="{D102E08B-F339-41A7-8779-8E498408C686}">
+    <filterColumn colId="1">
+      <customFilters>
+        <customFilter val="*vin*"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{AF0208C4-E4FE-4DFD-BAF4-BF1165EEA465}" name="STT" dataDxfId="41" dataCellStyle="Normal"/>
     <tableColumn id="2" xr3:uid="{CDE784D9-BEC1-45FE-9CFA-FBFFA9772F9D}" name="HỌ TÊN" dataDxfId="40" dataCellStyle="Normal"/>
@@ -3655,7 +3713,7 @@
   <dimension ref="B2:M55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="I18" sqref="I8:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,7 +3803,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -3812,7 +3870,7 @@
       <c r="L8" s="27"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3846,7 +3904,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3914,7 +3972,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3948,7 +4006,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3981,7 +4039,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4015,7 +4073,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4049,7 +4107,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4083,7 +4141,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -4151,7 +4209,7 @@
       <c r="L18" s="2"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -4185,7 +4243,7 @@
       <c r="L19" s="32"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4202,7 +4260,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4219,7 +4277,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -4241,7 +4299,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -4363,7 +4421,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B3:K3"/>
@@ -4383,8 +4440,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A2:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4392,9 +4449,9 @@
     <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" style="1" customWidth="1"/>
@@ -4423,7 +4480,7 @@
     </row>
     <row r="3" spans="2:16" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
@@ -4596,13 +4653,13 @@
       <c r="H10" s="53"/>
       <c r="I10" s="53"/>
       <c r="J10" s="60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K10" s="59" t="s">
         <v>86</v>
       </c>
       <c r="L10" s="60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M10" s="56"/>
     </row>
@@ -4939,16 +4996,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" s="3">
         <v>70081001153</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>83</v>
@@ -4968,16 +5025,16 @@
         <v>17</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E23" s="3">
         <v>27068001194</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>82</v>
@@ -5148,7 +5205,7 @@
   <dimension ref="A2:M56"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="A17:XFD17"/>
+      <selection activeCell="I8" sqref="I8:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5238,7 +5295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -5306,7 +5363,7 @@
       <c r="L8" s="35"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -5339,7 +5396,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B24" si="0">B9 +1</f>
         <v>4</v>
@@ -5409,7 +5466,7 @@
       <c r="L11" s="35"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5443,7 +5500,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -5479,7 +5536,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5513,7 +5570,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -5547,7 +5604,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -5581,7 +5638,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -5620,7 +5677,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>28</v>
@@ -5649,7 +5706,7 @@
       <c r="L18" s="35"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -5718,7 +5775,7 @@
       <c r="L20" s="35"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>71</v>
       </c>
@@ -5727,7 +5784,7 @@
         <v>15</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>76</v>
@@ -5755,7 +5812,7 @@
       <c r="L21" s="35"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -5788,7 +5845,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -5821,7 +5878,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -5981,7 +6038,7 @@
   <dimension ref="A2:M56"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+      <selection activeCell="I8" sqref="I8:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6071,7 +6128,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -6138,7 +6195,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -6171,7 +6228,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B24" si="0">B9 +1</f>
         <v>4</v>
@@ -6243,7 +6300,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6277,7 +6334,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6313,7 +6370,7 @@
       <c r="L13" s="35"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6346,7 +6403,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6380,7 +6437,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6414,7 +6471,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -6454,7 +6511,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>28</v>
@@ -6483,7 +6540,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -6550,7 +6607,7 @@
       <c r="L20" s="43"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f>B20 +1</f>
@@ -6584,7 +6641,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -6617,7 +6674,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6650,7 +6707,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -6809,7 +6866,7 @@
   <dimension ref="A2:M56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I8" sqref="I8:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6899,7 +6956,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -6968,7 +7025,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f>B8 +1</f>
         <v>3</v>
@@ -7001,7 +7058,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" ref="B10:B23" si="0">B9 +1</f>
         <v>4</v>
@@ -7072,7 +7129,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7106,7 +7163,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7142,7 +7199,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7176,7 +7233,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7210,7 +7267,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -7244,7 +7301,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7316,7 +7373,7 @@
       </c>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7384,7 +7441,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f>B20 +1</f>
@@ -7418,7 +7475,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7451,7 +7508,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7484,7 +7541,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -7624,7 +7681,7 @@
   <dimension ref="A2:M56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I8" sqref="I8:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7714,7 +7771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -7782,7 +7839,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7815,7 +7872,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7887,7 +7944,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7921,7 +7978,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7956,7 +8013,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7990,7 +8047,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8024,7 +8081,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8057,7 +8114,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8126,7 +8183,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -8193,7 +8250,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -8228,7 +8285,7 @@
       <c r="L21" s="2"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8261,7 +8318,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8294,7 +8351,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -8437,7 +8494,7 @@
   <dimension ref="A2:M56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I21"/>
+      <selection activeCell="I8" sqref="I8:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8527,7 +8584,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -8596,7 +8653,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -8630,7 +8687,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8702,7 +8759,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8736,7 +8793,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8772,7 +8829,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8806,7 +8863,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8840,7 +8897,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -8874,7 +8931,7 @@
       <c r="L16" s="35"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8945,7 +9002,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9012,7 +9069,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -9047,7 +9104,7 @@
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -9080,7 +9137,7 @@
       <c r="L22" s="2"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -9113,7 +9170,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -9346,7 +9403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -9402,7 +9459,7 @@
         <v>2040000</v>
       </c>
       <c r="I8" s="10">
-        <f t="shared" ref="I8:I22" si="1">H8*$E$26</f>
+        <f t="shared" ref="I8:I21" si="1">H8*$E$26</f>
         <v>1224000</v>
       </c>
       <c r="J8" s="47" t="s">
@@ -9414,7 +9471,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -9448,7 +9505,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -9520,7 +9577,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -9554,7 +9611,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -9590,7 +9647,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -9624,7 +9681,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -9658,7 +9715,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -9692,7 +9749,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -9760,7 +9817,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -9828,7 +9885,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -9869,7 +9926,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>6</v>
@@ -9887,8 +9944,7 @@
         <v>930000</v>
       </c>
       <c r="I22" s="10">
-        <f t="shared" si="1"/>
-        <v>558000</v>
+        <v>540000</v>
       </c>
       <c r="J22" s="47" t="s">
         <v>26</v>
@@ -9903,7 +9959,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>6</v>
@@ -9930,7 +9986,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -9970,7 +10026,7 @@
       <c r="I27" s="64"/>
       <c r="J27" s="9">
         <f>SUM(I7:I1001)</f>
-        <v>18630000</v>
+        <v>18612000</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -10073,7 +10129,7 @@
   <dimension ref="A2:P59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I21"/>
+      <selection activeCell="I8" sqref="I8:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10112,7 +10168,7 @@
     </row>
     <row r="3" spans="2:16" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
@@ -10168,7 +10224,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -10242,7 +10298,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -10276,7 +10332,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -10348,7 +10404,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -10382,7 +10438,7 @@
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -10418,7 +10474,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -10452,7 +10508,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -10486,7 +10542,7 @@
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
-    <row r="16" spans="2:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -10520,7 +10576,7 @@
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
-    <row r="17" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -10589,7 +10645,7 @@
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -10657,7 +10713,7 @@
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="3">
         <f t="shared" si="0"/>
@@ -10698,16 +10754,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" s="3">
         <v>70081001153</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>83</v>
@@ -10732,16 +10788,16 @@
         <v>17</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E23" s="3">
         <v>27068001194</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>82</v>
@@ -10760,7 +10816,7 @@
       <c r="L23" s="2"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="16.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -10893,7 +10949,6 @@
     </row>
     <row r="59" spans="2:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="B3:K3"/>
@@ -10914,8 +10969,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A2:P59"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10954,7 +11009,7 @@
     </row>
     <row r="3" spans="2:16" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B3" s="62" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="63"/>
       <c r="D3" s="63"/>
@@ -11354,11 +11409,11 @@
         <v>0</v>
       </c>
       <c r="J16" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K16" s="55"/>
       <c r="L16" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M16" s="12"/>
     </row>
@@ -11466,7 +11521,7 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="3">
         <f t="shared" si="0"/>
@@ -11493,11 +11548,13 @@
       <c r="I20" s="10">
         <v>875000</v>
       </c>
-      <c r="J20" s="45" t="s">
-        <v>72</v>
+      <c r="J20" s="47" t="s">
+        <v>26</v>
       </c>
       <c r="K20" s="35"/>
-      <c r="L20" s="12"/>
+      <c r="L20" s="65" t="s">
+        <v>115</v>
+      </c>
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -11541,16 +11598,16 @@
         <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E22" s="3">
         <v>70081001153</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>83</v>
@@ -11574,16 +11631,16 @@
         <v>17</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="E23" s="3">
         <v>27068001194</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>82</v>

</xml_diff>